<commit_message>
Test Cases after modification
</commit_message>
<xml_diff>
--- a/Validation/Test Cases.xlsx
+++ b/Validation/Test Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>TC ID</t>
   </si>
@@ -40,17 +40,10 @@
     <t>TC_1</t>
   </si>
   <si>
-    <t xml:space="preserve"> validate happy scenario</t>
+    <t xml:space="preserve"> validate button pressing</t>
   </si>
   <si>
-    <t>Run the Blender to see its behavior in normal state with normal voltage (5v-9v)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-1-The switch is to be connected to  the microcontroller.
-2- The Motor Driver is connected to microcontroller.
-3- The Motor is connected to the Motor Driver.
-4- Motor Driver and Microcontroller are  to be connected to Voltage Protection Circuit to Power Supply.</t>
+    <t>when pressing the button the state of blender must be changed from off to be speed 1 in normal state with normal voltage (5v-9v)</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -58,10 +51,43 @@
 2- watch motor rotational speed</t>
   </si>
   <si>
-    <t xml:space="preserve"> The blender start in off Mode then by every pressing the speed should be changed from speed 1 to speed 2 to speed 3 then finally return back to 0ff</t>
+    <t xml:space="preserve"> The blender start in off Mode then by pressing  button the speed should be changed from off to speed 1 then by every pressing  the speed changed from current to hiegher speed </t>
   </si>
   <si>
     <t>TC_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  when measuring  speed must be equivalent to speed 1</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 2</t>
+  </si>
+  <si>
+    <t>when pressing the button the state of blender must be changed from speed1 to be speed 2 in normal state with normal voltage (5v-9v)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  when measuring  speed must be equivalent to speed 2</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> validate Speed 3</t>
+  </si>
+  <si>
+    <t>when pressing the button the state of blender must be changed from speed 2 to be speed 3 in normal state with normal voltage (5v-9v)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  when measuring  speed must be equivalent to speed 3</t>
+  </si>
+  <si>
+    <t>TC_5</t>
   </si>
   <si>
     <t>Validate Pressing on button frequently.</t>
@@ -76,7 +102,7 @@
     <t>The button should not response to another action/pressing while the pressing in 1 second or less</t>
   </si>
   <si>
-    <t>TC_3</t>
+    <t>TC_6</t>
   </si>
   <si>
     <t>Validate Long Press on the button.</t>
@@ -93,7 +119,7 @@
     <t>The state/ speed should not be changed to other</t>
   </si>
   <si>
-    <t>TC_4</t>
+    <t>TC_7</t>
   </si>
   <si>
     <t>validate motor rotation</t>
@@ -106,7 +132,7 @@
 2- watch motor rotational direction</t>
   </si>
   <si>
-    <t>TC_5</t>
+    <t>TC_8</t>
   </si>
   <si>
     <t xml:space="preserve">Verify Protection circuit </t>
@@ -121,7 +147,7 @@
     <t>The system should shut down completely.</t>
   </si>
   <si>
-    <t>TC _6</t>
+    <t>TC _9</t>
   </si>
   <si>
     <t xml:space="preserve">Verify the PWM Voltage </t>
@@ -138,7 +164,7 @@
     <t>The PWM voltage should differ from speed to another.</t>
   </si>
   <si>
-    <t>TC_7</t>
+    <t>TC_10</t>
   </si>
   <si>
     <t>Verify the initial state of the blender.</t>
@@ -155,7 +181,7 @@
     <t>The initial state should be OFF and the motor speed should be zero.</t>
   </si>
   <si>
-    <t>TC_8</t>
+    <t>TC_11</t>
   </si>
   <si>
     <t>Verify No Power Button.</t>
@@ -373,63 +399,111 @@
       <c r="AA1" s="9"/>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3">
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4">
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
     <row r="6">
+      <c r="A6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
     <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
@@ -446,25 +520,25 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
@@ -481,25 +555,25 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17">
+      <c r="A17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
@@ -520,106 +594,111 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23">
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="A23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="14"/>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="I24" s="14"/>
     </row>
     <row r="25">
       <c r="I25" s="14"/>
     </row>
     <row r="26">
-      <c r="I26" s="14"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27">
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="16"/>
-      <c r="C31" s="15"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="10" t="s">
+      <c r="A27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B27" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>46</v>
       </c>
+      <c r="F27" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" s="16"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33">
-      <c r="B33" s="16"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="15"/>
       <c r="D33" s="13"/>
       <c r="E33" s="16"/>
@@ -628,7 +707,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34">
-      <c r="B34" s="18"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="15"/>
       <c r="D34" s="13"/>
       <c r="E34" s="16"/>
@@ -637,11 +716,11 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35">
-      <c r="B35" s="16"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="16"/>
-      <c r="F35" s="15"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
@@ -9348,43 +9427,29 @@
       <c r="G1002" s="13"/>
       <c r="H1002" s="13"/>
     </row>
-    <row r="1003">
-      <c r="B1003" s="18"/>
-      <c r="C1003" s="13"/>
-      <c r="D1003" s="13"/>
-      <c r="E1003" s="16"/>
-      <c r="F1003" s="13"/>
-      <c r="G1003" s="13"/>
-      <c r="H1003" s="13"/>
-    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="D2:D32"/>
+  <mergeCells count="21">
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D2:D31"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>